<commit_message>
Adding PNR Information Logic
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>TC Count</t>
   </si>
@@ -27,6 +27,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>PNR Information</t>
+  </si>
+  <si>
+    <t>J5F8JX</t>
   </si>
 </sst>
 </file>
@@ -87,6 +93,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -98,6 +107,9 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
updating PNR Information Logic
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>TC Count</t>
   </si>
@@ -29,10 +29,43 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>PNR Information</t>
+    <t>Flight Number</t>
+  </si>
+  <si>
+    <t>PNR Number</t>
+  </si>
+  <si>
+    <t>PNR Validity</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>FR 202</t>
+  </si>
+  <si>
+    <t>OTME5P</t>
+  </si>
+  <si>
+    <t>Fri 06 Dec 2019</t>
+  </si>
+  <si>
+    <t>DUBLIN</t>
+  </si>
+  <si>
+    <t>LONDON STANSTED</t>
+  </si>
+  <si>
+    <t>AL 1235</t>
   </si>
   <si>
     <t>Booking Failed</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -96,6 +129,18 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -108,7 +153,45 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>